<commit_message>
Departure Date Return Date Round Trip
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
   <si>
     <t>TestCase</t>
   </si>
@@ -50,12 +50,30 @@
     <t>Input To</t>
   </si>
   <si>
+    <t>Multi From 2</t>
+  </si>
+  <si>
+    <t>Multi To 2</t>
+  </si>
+  <si>
+    <t>Multi From 3</t>
+  </si>
+  <si>
+    <t>Multi To 3</t>
+  </si>
+  <si>
     <t>Departure Date</t>
   </si>
   <si>
     <t>Return Date</t>
   </si>
   <si>
+    <t>Multi Departure 2</t>
+  </si>
+  <si>
+    <t>Multi Departure 3</t>
+  </si>
+  <si>
     <t>Airline Input</t>
   </si>
   <si>
@@ -86,23 +104,42 @@
     <t>Attachments</t>
   </si>
   <si>
+    <t>OneWay</t>
+  </si>
+  <si>
     <t>25/09/2025</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi nhập các 
+thông tin hợp lệ</t>
+  </si>
+  <si>
+    <t>Agency đã login thành công</t>
+  </si>
+  <si>
+    <t>one-way</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>27/09/2025</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>Hiện form danh sách chuyến bay</t>
   </si>
   <si>
     <t>Kiểm tra trường nơi đi khi
 không nhập dữ liệu gì</t>
   </si>
   <si>
-    <t>Agency đã login thành công</t>
-  </si>
-  <si>
-    <t>one-way</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>business</t>
+    <t>20/10/2025</t>
   </si>
   <si>
     <t>Trường này là bắt buộc!</t>
@@ -116,19 +153,29 @@
 trước ngày hiện tại</t>
   </si>
   <si>
-    <t>Seoul</t>
-  </si>
-  <si>
     <t>Không cho phép chọn</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi nhập nơi đi
+trùng nơi đến</t>
+  </si>
+  <si>
+    <t>Round Trip</t>
+  </si>
+  <si>
+    <t>29/09/2025</t>
+  </si>
+  <si>
+    <t>round-trip</t>
+  </si>
+  <si>
+    <t>26/09/2025</t>
   </si>
   <si>
     <t>Kiểm tra chọn ngày về
 trước ngày hiện tại</t>
   </si>
   <si>
-    <t>round-trip</t>
-  </si>
-  <si>
     <t>Kiểm tra chọn ngày đi 
 trùng với ngày về</t>
   </si>
@@ -136,7 +183,33 @@
     <t>economy</t>
   </si>
   <si>
-    <t>Hiện form danh sách chuyến bay</t>
+    <t>Multi Trip</t>
+  </si>
+  <si>
+    <t>multi-city</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#multi_from_3"}
+  (Session info: chrome=140.0.7339.186)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.35.0', revision: '1c58e5028b'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.8'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [aeed1c9ad56033c8bc77715d94629792, findElement {using=id, value=multi_from_3}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 140.0.7339.186, chrome: {chromedriverVersion: 140.0.7339.207 (17230b545fd..., userDataDir: C:\Users\Admin\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:54875}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:54875/devtoo..., se:cdpVersion: 140.0.7339.186, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: aeed1c9ad56033c8bc77715d94629792</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -310,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +398,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -510,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -522,6 +601,43 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -655,7 +771,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,119 +783,119 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -790,10 +906,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1115,35 +1243,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="P1" sqref="P$1:P$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.5555555555556" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.4444444444444" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.8888888888889" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.1111111111111" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.3333333333333" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.4444444444444" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1111111111111" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.6666666666667" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.3333333333333" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.5555555555556" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.8888888888889" style="2" customWidth="1"/>
-    <col min="12" max="13" width="17.5555555555556" style="2" customWidth="1"/>
-    <col min="14" max="15" width="36" style="2" customWidth="1"/>
-    <col min="16" max="16" width="31" style="2" customWidth="1"/>
-    <col min="17" max="17" width="23.8888888888889" style="2" customWidth="1"/>
-    <col min="18" max="18" width="27.6666666666667" style="2" customWidth="1"/>
-    <col min="19" max="19" width="30.7777777777778" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="16.5555555555556"/>
+    <col min="2" max="2" customWidth="true" style="2" width="23.4444444444444"/>
+    <col min="3" max="3" customWidth="true" style="2" width="23.8888888888889"/>
+    <col min="4" max="4" customWidth="true" style="2" width="28.1111111111111"/>
+    <col min="5" max="5" customWidth="true" style="2" width="15.3333333333333"/>
+    <col min="6" max="6" customWidth="true" style="2" width="19.4444444444444"/>
+    <col min="7" max="7" customWidth="true" style="2" width="18.1111111111111"/>
+    <col min="8" max="12" customWidth="true" style="2" width="19.6666666666667"/>
+    <col min="13" max="13" customWidth="true" style="2" width="16.3333333333333"/>
+    <col min="14" max="15" customWidth="true" style="2" width="18.3333333333333"/>
+    <col min="16" max="16" customWidth="true" style="2" width="15.5555555555556"/>
+    <col min="17" max="17" customWidth="true" style="2" width="18.8888888888889"/>
+    <col min="18" max="19" customWidth="true" style="2" width="17.5555555555556"/>
+    <col min="20" max="21" customWidth="true" style="2" width="36.0"/>
+    <col min="22" max="22" customWidth="true" style="2" width="31.0"/>
+    <col min="23" max="23" customWidth="true" style="2" width="23.8888888888889"/>
+    <col min="24" max="24" customWidth="true" style="2" width="27.6666666666667"/>
+    <col min="25" max="25" customWidth="true" style="2" width="30.7777777777778"/>
+    <col min="26" max="16384" style="2" width="9.0"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:19">
+    <row r="1" s="1" customFormat="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1201,233 +1330,648 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" ht="46" customHeight="1" spans="1:19">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4">
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:25">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="9"/>
+    </row>
+    <row r="3" ht="46" customHeight="1" spans="1:25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="M2" s="4">
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1</v>
+      </c>
+      <c r="S3" s="6">
         <v>0</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="T3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
     </row>
-    <row r="3" ht="46" customHeight="1" spans="1:19">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="4" ht="46" customHeight="1" spans="1:25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4">
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6">
+        <v>1</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" ht="46" customHeight="1" spans="1:25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="C5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="6">
         <v>0</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="T5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
     </row>
-    <row r="4" ht="46" customHeight="1" spans="1:19">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" ht="46" customHeight="1" spans="1:25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>1</v>
+      </c>
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" ht="48" customHeight="1" spans="1:25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="6">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6">
+        <v>0</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="30" customHeight="1" spans="1:25">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="9"/>
+    </row>
+    <row r="9" ht="46" customHeight="1" spans="1:25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="4">
-        <v>24</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6">
+        <v>1</v>
+      </c>
+      <c r="R9" s="6">
+        <v>1</v>
+      </c>
+      <c r="S9" s="6">
         <v>0</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="T9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
     </row>
-    <row r="5" ht="46" customHeight="1" spans="1:19">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="10" ht="46" customHeight="1" spans="1:25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="G10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6">
+        <v>1</v>
+      </c>
+      <c r="R10" s="6">
+        <v>1</v>
+      </c>
+      <c r="S10" s="6">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" ht="46" customHeight="1" spans="1:25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="4">
-        <v>25</v>
-      </c>
-      <c r="I5" s="4">
-        <v>24</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="E11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="6">
+        <v>1</v>
+      </c>
+      <c r="S11" s="6">
         <v>0</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="T11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
     </row>
-    <row r="6" ht="46" customHeight="1" spans="1:19">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    <row r="12" ht="46" customHeight="1" spans="1:25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="M12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6">
+        <v>1</v>
+      </c>
+      <c r="R12" s="6">
+        <v>1</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="30" customHeight="1" spans="1:25">
+      <c r="A13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="9"/>
+    </row>
+    <row r="14" ht="49" customHeight="1" spans="1:25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="4">
-        <v>25</v>
-      </c>
-      <c r="I6" s="4">
-        <v>25</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="H14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O14" s="8">
+        <v>45787</v>
+      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6">
+        <v>1</v>
+      </c>
+      <c r="R14" s="6">
+        <v>1</v>
+      </c>
+      <c r="S14" s="6">
         <v>0</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="4" t="s">
+      <c r="T14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="V14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A8:Y8"/>
+    <mergeCell ref="A13:Y13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Format Function Select Date
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>TestCase</t>
   </si>
@@ -180,6 +180,9 @@
 trùng với ngày về</t>
   </si>
   <si>
+    <t>30/09/2025</t>
+  </si>
+  <si>
     <t>economy</t>
   </si>
   <si>
@@ -193,20 +196,6 @@
   </si>
   <si>
     <t>Singapore</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#multi_from_3"}
-  (Session info: chrome=140.0.7339.186)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.35.0', revision: '1c58e5028b'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.8'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [aeed1c9ad56033c8bc77715d94629792, findElement {using=id, value=multi_from_3}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 140.0.7339.186, chrome: {chromedriverVersion: 140.0.7339.207 (17230b545fd..., userDataDir: C:\Users\Admin\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:54875}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:54875/devtoo..., se:cdpVersion: 140.0.7339.186, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: aeed1c9ad56033c8bc77715d94629792</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Pass</t>
@@ -895,7 +884,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -917,9 +906,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1245,8 +1231,8 @@
   <sheetPr/>
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="P1" sqref="P$1:P$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12:W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1376,7 +1362,7 @@
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
-      <c r="Y2" s="9"/>
+      <c r="Y2" s="8"/>
     </row>
     <row r="3" ht="46" customHeight="1" spans="1:25">
       <c r="A3" s="6"/>
@@ -1656,7 +1642,7 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
-      <c r="Y8" s="9"/>
+      <c r="Y8" s="8"/>
     </row>
     <row r="9" ht="46" customHeight="1" spans="1:25">
       <c r="A9" s="6"/>
@@ -1842,10 +1828,10 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -1860,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U12" s="6" t="s">
         <v>34</v>
@@ -1872,7 +1858,7 @@
     </row>
     <row r="13" s="1" customFormat="1" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1897,7 +1883,7 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
-      <c r="Y13" s="9"/>
+      <c r="Y13" s="8"/>
     </row>
     <row r="14" ht="49" customHeight="1" spans="1:25">
       <c r="A14" s="6"/>
@@ -1911,7 +1897,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>30</v>
@@ -1923,13 +1909,13 @@
         <v>31</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>32</v>
@@ -1938,8 +1924,8 @@
       <c r="N14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="8">
-        <v>45787</v>
+      <c r="O14" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6">
@@ -1952,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U14" s="6" t="s">
         <v>34</v>
@@ -1961,7 +1947,7 @@
         <v>34</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>

</xml_diff>

<commit_message>
Contact Info (Not Done Select Date)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -122,13 +122,13 @@
     <t>one-way</t>
   </si>
   <si>
+    <t>Singapore</t>
+  </si>
+  <si>
     <t>Manila</t>
   </si>
   <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>02/10/2025</t>
+    <t>04/10/2025</t>
   </si>
   <si>
     <t>economy</t>
@@ -186,6 +186,9 @@
     <t>Kuala Lumpur</t>
   </si>
   <si>
+    <t>02/10/2025</t>
+  </si>
+  <si>
     <t>07/10/2025</t>
   </si>
   <si>
@@ -210,9 +213,6 @@
   </si>
   <si>
     <t>01/10/2025</t>
-  </si>
-  <si>
-    <t>04/10/2025</t>
   </si>
   <si>
     <t>05/10/2025</t>
@@ -1501,8 +1501,8 @@
   <sheetPr/>
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1666,10 +1666,10 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="16">
         <v>0</v>
@@ -1936,17 +1936,17 @@
         <v>49</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="21" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -1999,7 +1999,7 @@
         <v>43</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
@@ -2030,7 +2030,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>28</v>
@@ -2049,7 +2049,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M11" s="16" t="s">
         <v>43</v>
@@ -2083,7 +2083,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>28</v>
@@ -2102,10 +2102,10 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="13" s="11" customFormat="1" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -2171,10 +2171,10 @@
         <v>28</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>49</v>
@@ -2183,20 +2183,20 @@
         <v>49</v>
       </c>
       <c r="I14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="L14" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M14" s="16"/>
       <c r="N14" s="21" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>59</v>
@@ -2241,8 +2241,8 @@
   <sheetPr/>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -2341,7 +2341,7 @@
         <v>67</v>
       </c>
       <c r="E3" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:15">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>

</xml_diff>

<commit_message>
Format Write Testcase, TestResult - Fix FLight List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="66">
   <si>
     <t>TestCase</t>
   </si>
@@ -109,7 +109,7 @@
     <t>OneWay</t>
   </si>
   <si>
-    <t>29/09/2025</t>
+    <t>30/09/2025</t>
   </si>
   <si>
     <t>Kiểm tra khi nhập các 
@@ -122,34 +122,25 @@
     <t>one-way</t>
   </si>
   <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Manila</t>
-  </si>
-  <si>
-    <t>04/10/2025</t>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>23/10/2025</t>
   </si>
   <si>
     <t>economy</t>
   </si>
   <si>
     <t>Hiện form danh sách chuyến bay</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>Kiểm tra trường nơi đi khi
 không nhập dữ liệu gì</t>
   </si>
   <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>20/10/2025</t>
-  </si>
-  <si>
     <t>Trường này là bắt buộc!</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
 trước ngày hiện tại</t>
   </si>
   <si>
-    <t>Seoul</t>
-  </si>
-  <si>
     <t>25/09/2025</t>
   </si>
   <si>
@@ -174,25 +162,19 @@
 trùng nơi đến</t>
   </si>
   <si>
-    <t>27/09/2025</t>
-  </si>
-  <si>
     <t>Round Trip</t>
   </si>
   <si>
     <t>round-trip</t>
   </si>
   <si>
-    <t>Kuala Lumpur</t>
-  </si>
-  <si>
-    <t>02/10/2025</t>
-  </si>
-  <si>
-    <t>07/10/2025</t>
-  </si>
-  <si>
-    <t>26/09/2025</t>
+    <t>03/12/2025</t>
+  </si>
+  <si>
+    <t>05/12/2025</t>
+  </si>
+  <si>
+    <t>27/10/2025</t>
   </si>
   <si>
     <t>Kiểm tra chọn ngày về
@@ -203,19 +185,25 @@
 trùng với ngày về</t>
   </si>
   <si>
-    <t>30/09/2025</t>
-  </si>
-  <si>
     <t>Multi Trip</t>
   </si>
   <si>
     <t>multi-city</t>
   </si>
   <si>
-    <t>01/10/2025</t>
-  </si>
-  <si>
-    <t>05/10/2025</t>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>29/10/2025</t>
+  </si>
+  <si>
+    <t>31/10/2025</t>
   </si>
   <si>
     <t>OneWay Index</t>
@@ -1178,6 +1166,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1501,8 +1492,8 @@
   <sheetPr/>
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1680,12 +1671,8 @@
       <c r="U3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>35</v>
-      </c>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
       <c r="X3" s="16"/>
       <c r="Y3" s="16"/>
     </row>
@@ -1695,7 +1682,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -1705,14 +1692,14 @@
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
-      <c r="L4" s="16" t="s">
-        <v>38</v>
+      <c r="L4" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -1731,7 +1718,7 @@
         <v>33</v>
       </c>
       <c r="U4" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
@@ -1744,7 +1731,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>28</v>
@@ -1753,15 +1740,15 @@
         <v>29</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
-      <c r="L5" s="16" t="s">
-        <v>38</v>
+      <c r="L5" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
@@ -1780,7 +1767,7 @@
         <v>33</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
@@ -1793,7 +1780,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>28</v>
@@ -1802,17 +1789,17 @@
         <v>29</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
@@ -1831,7 +1818,7 @@
         <v>33</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
@@ -1844,7 +1831,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>28</v>
@@ -1853,17 +1840,17 @@
         <v>29</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
-        <v>46</v>
+      <c r="L7" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
@@ -1891,7 +1878,7 @@
     </row>
     <row r="8" s="11" customFormat="1" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -1930,10 +1917,10 @@
         <v>28</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>31</v>
@@ -1942,11 +1929,11 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>51</v>
+      <c r="L9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -1977,29 +1964,29 @@
         <v>26</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
@@ -2017,7 +2004,7 @@
         <v>33</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
@@ -2030,29 +2017,29 @@
         <v>26</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="16" t="s">
-        <v>52</v>
+      <c r="L11" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -2070,7 +2057,7 @@
         <v>33</v>
       </c>
       <c r="U11" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="V11" s="17"/>
       <c r="W11" s="16"/>
@@ -2083,29 +2070,29 @@
         <v>26</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>55</v>
+      <c r="L12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -2132,7 +2119,7 @@
     </row>
     <row r="13" s="11" customFormat="1" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -2171,35 +2158,35 @@
         <v>28</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="L14" s="21" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="M14" s="16"/>
       <c r="N14" s="21" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P14" s="16"/>
       <c r="Q14" s="16">
@@ -2231,7 +2218,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="L4:L7 L10:M12" twoDigitTextYear="1"/>
+    <ignoredError sqref="L6 M11" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2241,8 +2228,8 @@
   <sheetPr/>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -2277,22 +2264,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>20</v>
@@ -2331,17 +2318,17 @@
     </row>
     <row r="3" ht="43.2" spans="1:15">
       <c r="A3" s="7"/>
-      <c r="B3" s="8">
-        <v>45929</v>
+      <c r="B3" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E3" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2356,7 +2343,7 @@
     </row>
     <row r="4" customHeight="1" spans="1:15">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
@@ -2375,14 +2362,14 @@
     </row>
     <row r="5" ht="43.2" spans="1:15">
       <c r="A5" s="7"/>
-      <c r="B5" s="8">
-        <v>45929</v>
+      <c r="B5" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10">
@@ -2402,7 +2389,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:15">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
@@ -2421,20 +2408,20 @@
     </row>
     <row r="7" ht="43.2" spans="1:15">
       <c r="A7" s="7"/>
-      <c r="B7" s="8">
-        <v>45929</v>
+      <c r="B7" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
Fix Date Search Flight Write Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -155,7 +155,7 @@
     <t>25/09/2025</t>
   </si>
   <si>
-    <t>Không cho phép chọn</t>
+    <t>Không cho phép chọn 25/09/2025</t>
   </si>
   <si>
     <t>Kiểm tra khi nhập nơi đi
@@ -1492,8 +1492,8 @@
   <sheetPr/>
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3:W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2056,7 +2056,7 @@
       <c r="T11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="17" t="s">
         <v>40</v>
       </c>
       <c r="V11" s="17"/>

</xml_diff>